<commit_message>
add final facts set and update tests
</commit_message>
<xml_diff>
--- a/tests/data/Dennsen86_stats_2024-06-15_REFERENCE.xlsx
+++ b/tests/data/Dennsen86_stats_2024-06-15_REFERENCE.xlsx
@@ -1,29 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a8b0bd3a772d8ada/Dokumente/Projekte/alttpr/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="11_337515925B70DB01DB783C11595ED87656CDFF39" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8BF5E754-F838-477F-9387-0350F815CBB9}"/>
+  <xr:revisionPtr revIDLastSave="26" documentId="11_337515925B70DB01DB783C11595ED87656CDFF39" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B8C38EFC-1E40-463E-83A2-308AF6D41B53}"/>
   <bookViews>
-    <workbookView xWindow="-19305" yWindow="0" windowWidth="19410" windowHeight="10545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$45</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$44</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="52">
   <si>
     <t>Kategorie</t>
   </si>
@@ -125,9 +125,6 @@
   </si>
   <si>
     <t>Blitzschnell! Der Median aller ALttPR Community-/Weekly-Race-Zeiten von Dennsen86 liegt bei 01:39:29</t>
-  </si>
-  <si>
-    <t>Von wegen Safe Letzter! In 105 ALttPR Community-/Weekly-Races war Dennsen86 auf dem 3. bis 8. Platz! Das sind 48% von insgesamt 217 Races</t>
   </si>
   <si>
     <t>Ragequit, Stromausfall oder BSG?! 42 ALttPR Community-/Weekly-Races hat Dennsen86 nicht beendet! Das sind 19% von insgesamt 217 Races</t>
@@ -203,12 +200,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -238,10 +241,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -545,25 +557,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C45"/>
+  <dimension ref="A1:C44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="17.42578125" customWidth="1"/>
+    <col min="3" max="3" width="133.7109375" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
@@ -574,18 +587,18 @@
       <c r="B2" t="s">
         <v>23</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>10002</v>
       </c>
       <c r="B3" t="s">
         <v>23</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="4" t="s">
         <v>25</v>
       </c>
     </row>
@@ -593,15 +606,15 @@
       <c r="B4" t="s">
         <v>23</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>23</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="4" t="s">
         <v>27</v>
       </c>
     </row>
@@ -609,7 +622,7 @@
       <c r="B6" t="s">
         <v>23</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="4" t="s">
         <v>28</v>
       </c>
     </row>
@@ -617,7 +630,7 @@
       <c r="B7" t="s">
         <v>23</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="4" t="s">
         <v>29</v>
       </c>
     </row>
@@ -625,7 +638,7 @@
       <c r="B8" t="s">
         <v>23</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="4" t="s">
         <v>30</v>
       </c>
     </row>
@@ -633,15 +646,15 @@
       <c r="B9" t="s">
         <v>23</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>23</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="4" t="s">
         <v>32</v>
       </c>
     </row>
@@ -649,7 +662,7 @@
       <c r="B11" t="s">
         <v>23</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="4" t="s">
         <v>33</v>
       </c>
     </row>
@@ -657,7 +670,7 @@
       <c r="B12" t="s">
         <v>23</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="3" t="s">
         <v>34</v>
       </c>
     </row>
@@ -665,15 +678,15 @@
       <c r="B13" t="s">
         <v>23</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>23</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="4" t="s">
         <v>36</v>
       </c>
     </row>
@@ -681,31 +694,31 @@
       <c r="B15" t="s">
         <v>23</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>23</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>23</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>23</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="4" t="s">
         <v>40</v>
       </c>
     </row>
@@ -713,7 +726,7 @@
       <c r="B19" t="s">
         <v>23</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="4" t="s">
         <v>41</v>
       </c>
     </row>
@@ -721,211 +734,203 @@
       <c r="B20" t="s">
         <v>23</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="3" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>23</v>
-      </c>
-      <c r="C21" t="s">
         <v>43</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>44</v>
-      </c>
-      <c r="C22" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" s="4" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>44</v>
-      </c>
-      <c r="C23" t="s">
+        <v>43</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>44</v>
-      </c>
-      <c r="C24" t="s">
+        <v>43</v>
+      </c>
+      <c r="C24" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>44</v>
-      </c>
-      <c r="C25" t="s">
+        <v>43</v>
+      </c>
+      <c r="C25" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>44</v>
-      </c>
-      <c r="C26" t="s">
+        <v>43</v>
+      </c>
+      <c r="C26" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>44</v>
-      </c>
-      <c r="C27" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>2</v>
       </c>
-      <c r="C28" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C28" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>2</v>
       </c>
-      <c r="C29" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C29" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>2</v>
       </c>
-      <c r="C30" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C30" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>2</v>
-      </c>
-      <c r="C31" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>7</v>
-      </c>
-      <c r="C32" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>9</v>
-      </c>
-      <c r="C33" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>11</v>
       </c>
-      <c r="C34" t="s">
-        <v>12</v>
+      <c r="C34" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>11</v>
       </c>
-      <c r="C35" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C35" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>11</v>
       </c>
-      <c r="C36" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C36" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>11</v>
       </c>
-      <c r="C37" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C37" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>11</v>
       </c>
-      <c r="C38" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C38" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>11</v>
       </c>
-      <c r="C39" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C39" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>11</v>
       </c>
-      <c r="C40" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C40" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>11</v>
       </c>
-      <c r="C41" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C41" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>11</v>
       </c>
-      <c r="C42" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C42" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>11</v>
       </c>
-      <c r="C43" t="s">
-        <v>21</v>
+      <c r="C43" s="3" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="44" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>11</v>
-      </c>
-      <c r="C44" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B45" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C45" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C45">
-      <sortCondition ref="A1:A45"/>
+  <autoFilter ref="A1:C44" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C44">
+      <sortCondition ref="A1:A44"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>